<commit_message>
added the NER file deleted the article
</commit_message>
<xml_diff>
--- a/query_results.xlsx
+++ b/query_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,76 @@
         <v>1234</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDC"[Title/Abstract] OR hormonally active agents[Title/Abstract] OR Endocrine disrupting compounds) AND ("Receptors, Endocrine"[MeSH Terms] OR "receptors"[Title/Abstract] OR "receptor"[Title/Abstract]) AND ("binding"[Title/Abstract] OR "assay"[Title/Abstract] OR "experiment"[Title/Abstract]) NOT review[Publication Type]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDC"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) AND ("Receptors, Endocrine"[MeSH Terms] OR "receptors"[Title/Abstract] OR "receptor"[Title/Abstract]) AND ("binding"[Title/Abstract] OR "assay"[Title/Abstract] OR "experiment"[Title/Abstract]) NOT review[Publication Type] OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Bisphenol A"[MeSH Terms] OR "BPA"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Phthalates"[MeSH Terms] OR "Phthalate"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Polychlorinated Biphenyls"[MeSH Terms] OR "PCBs"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Regulation"[MeSH Terms] OR "Risk Assessment"[Title/Abstract]))</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5818</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDC"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) AND ("Receptors, Endocrine"[MeSH Terms] OR "receptors"[Title/Abstract] OR "receptor"[Title/Abstract]) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Bisphenol A"[MeSH Terms] OR "BPA"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Phthalates"[MeSH Terms] OR "Phthalate"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Polychlorinated Biphenyls"[MeSH Terms] OR "PCBs"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Regulation"[MeSH Terms] OR "Risk Assessment"[Title/Abstract]))</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>7295</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDC"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) AND ("Receptors, Endocrine"[MeSH Terms] OR "receptors"[Title/Abstract] OR "receptor"[Title/Abstract] OR target[Title/Abstract]) AND ("human estrogen receptor alpha"[Title/Abstract] OR  "HERa"[Title/Abstract] OR "Estrogen"[Title/Abstract] OR target[Title/Abstract]) OR "estradiol"[Title/Abstract]AND ("HERb"[Title/Abstract] OR "Human estrogen receptor beta"[Title/Abstract])AND ("binding"[Title/Abstract]AND ("Human andorgen receptor"[Title/Abstract] or "HAR"[Title/Abstract] or "Testosterone"[Title/Abstract])AND ("NR3C1"[Title/Abstract] OR "Human glucocorticoid receptor"[Title/Abstract]) OR  "Dexamethasone"[Title/Abstract]AND ("Human mineralcorticoid receptor"[Title/Abstract],"Aldosterone"[Title/Abstract], "NR3C2"[Tilte/Abstract]AND "Progesterone"[Title/Abstract] OR "NR3C3"[Title/Abstract] OR "Human progesterone receptor"[Title/Abstract] OR "Progesterone"[Title/Abstract]NOT review[Publication Type]OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Bisphenol A"[MeSH Terms] OR "BPA"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Phthalates"[MeSH Terms] OR "Phthalate"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Polychlorinated Biphenyls"[MeSH Terms] OR "PCBs"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Regulation"[MeSH Terms] OR "Risk Assessment"[Title/Abstract]))</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDC"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) AND (human"[Title/Abstract]")AND ("Receptors, Endocrine"[MeSH Terms] OR "receptors"[Title/Abstract] OR "receptor"[Title/Abstract] OR target[Title/Abstract]) AND ("human estrogen receptor alpha"[Title/Abstract] OR  "HERa"[Title/Abstract] OR "Estrogen"[Title/Abstract] OR target[Title/Abstract]) OR "estradiol"[Title/Abstract]AND ("HERb"[Title/Abstract] OR "Human estrogen receptor beta"[Title/Abstract])AND ("binding"[Title/Abstract]AND ("Human andorgen receptor"[Title/Abstract] or "HAR"[Title/Abstract] or "Testosterone"[Title/Abstract])AND ("NR3C1"[Title/Abstract] OR "Human glucocorticoid receptor"[Title/Abstract]) OR  "Dexamethasone"[Title/Abstract]AND ("Human mineralcorticoid receptor"[Title/Abstract],"Aldosterone"[Title/Abstract], "NR3C2"[Tilte/Abstract]AND "Progesterone"[Title/Abstract] OR "NR3C3"[Title/Abstract] OR "Human progesterone receptor"[Title/Abstract] OR "Progesterone"[Title/Abstract]NOT review[Publication Type]OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Bisphenol A"[MeSH Terms] OR "BPA"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Phthalates"[MeSH Terms] OR "Phthalate"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Polychlorinated Biphenyls"[MeSH Terms] OR "PCBs"[Title/Abstract])) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND ("Regulation"[MeSH Terms] OR "Risk Assessment"[Title/Abstract]))</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDCs"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) AND (human[Title/Abstract]) AND ("Receptors, Endocrine"[MeSH Terms] OR "receptors"[Title/Abstract] OR "receptor"[Title/Abstract] OR target[Title/Abstract]) AND (("human estrogen receptor alpha"[Title/Abstract] OR "HERa"[Title/Abstract] OR "Estrogen"[Title/Abstract] OR target[Title/Abstract]) OR "estradiol"[Title/Abstract] OR ("HERb"[Title/Abstract] OR "Human estrogen receptor beta"[Title/Abstract]) OR ("binding"[Title/Abstract] AND ("Human androgen receptor"[Title/Abstract] OR "HAR"[Title/Abstract] OR "Testosterone"[Title/Abstract])) OR ("NR3C1"[Title/Abstract] OR "Human glucocorticoid receptor"[Title/Abstract]) OR "Dexamethasone"[Title/Abstract] OR ("Human mineralocorticoid receptor"[Title/Abstract] OR "Aldosterone"[Title/Abstract] OR "NR3C2"[Title/Abstract]) OR ("Progesterone"[Title/Abstract] OR "NR3C3"[Title/Abstract] OR "Human progesterone receptor"[Title/Abstract]) ) AND (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND (("Bisphenol A"[MeSH Terms] OR "BPA"[Title/Abstract]) OR ("Phthalates"[MeSH Terms] OR "Phthalate"[Title/Abstract]) OR ("Polychlorinated Biphenyls"[MeSH Terms] OR "PCBs"[Title/Abstract]) OR ("Regulation"[MeSH Terms] OR "Risk Assessment"[Title/Abstract]) ) ) NOT review[Publication Type]</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDCs"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) AND (human[Title/Abstract]) AND ("Receptors, Endocrine"[MeSH Terms] OR "receptors"[Title/Abstract] OR "receptor"[Title/Abstract] OR target[Title/Abstract]) AND (("human estrogen receptor alpha"[Title/Abstract] OR "HERa"[Title/Abstract] OR "Estrogen"[Title/Abstract] OR target[Title/Abstract]) OR "estradiol"[Title/Abstract] OR ("HERb"[Title/Abstract] OR "Human estrogen receptor beta"[Title/Abstract]) OR ("binding"[Title/Abstract] AND ("Human androgen receptor"[Title/Abstract] OR "HAR"[Title/Abstract] OR "Testosterone"[Title/Abstract])) OR ("NR3C1"[Title/Abstract] OR "Human glucocorticoid receptor"[Title/Abstract]) OR "Dexamethasone"[Title/Abstract] OR ("Human mineralocorticoid receptor"[Title/Abstract] OR "Aldosterone"[Title/Abstract] OR "NR3C2"[Title/Abstract]) OR ("Progesterone"[Title/Abstract] OR "NR3C3"[Title/Abstract] OR "Human progesterone receptor"[Title/Abstract]) ) OR (("Endocrine Disrupting Chemicals"[MeSH Terms] OR "Endocrine Disruptors"[MeSH Terms] OR "EDCs"[Title/Abstract] OR "Endocrine Disruptors"[Title/Abstract]) AND (("Bisphenol A"[MeSH Terms] OR "BPA"[Title/Abstract]) OR ("Phthalates"[MeSH Terms] OR "Phthalate"[Title/Abstract]) OR ("Polychlorinated Biphenyls"[MeSH Terms] OR "PCBs"[Title/Abstract]) ) ) NOT review[Publication Type]</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
training set annotation and implementation on NER
</commit_message>
<xml_diff>
--- a/query_results.xlsx
+++ b/query_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,6 +583,26 @@
         <v>4360</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDCs"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) ) NOT review[Publication Type]AND Homo sapiens[MeSH Terms]AND ("Reproduction"[MeSH Terms] OR "Endocrine System"[MeSH Terms] OR "chemistry"[MeSH Terms] OR "toxicity"[MeSH Terms]OR "Disruptors, Endocrine"[MeSH Terms] OR "Endocrine Disruptor"[MeSH Terms] OR "Endocrine Disrupting Chemical"[MeSH Terms] OR "Chemical, Endocrine Disrupting"[MeSH Terms] OR "Disrupting Chemical, Endocrine"[MeSH Terms] OR "Endocrine Disruptor Effect"[MeSH Terms] OR "Endocrine Disruptor Effect"[MeSH Terms]OR "Water pollutants"[MeSH Terms] OR "Herbicides"[MeSH Terms] OR "Pesticides"[MeSH Terms] OR  "Gonadal Steroid Hormones"[MeSH Terms] OR "fertility"[MeSH Terms] OR "infertility"[MeSH Terms] OR "Androgen antagonists"[MeSH Terms] OR "astrogen antagonists"[MeSH Terms] OR "estrogen agonists"[MeSH Terms] OR "androgen agonists"[MeSH Terms]) </t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">("Endocrine Disruptors"[MeSH Terms] OR "endocrine disrupting chemicals"[Title/Abstract] OR "EDCs"[Title/Abstract] OR "hormonally active agents"[Title/Abstract] OR "Endocrine disrupting compounds"[Title/Abstract]) ) NOT review[Publication Type]AND ("Reproduction"[MeSH Terms] OR "Endocrine System"[MeSH Terms] OR "chemistry"[MeSH Terms] OR "toxicity"[MeSH Terms]OR "Disruptors, Endocrine"[MeSH Terms] OR "Endocrine Disruptor"[MeSH Terms] OR "Endocrine Disrupting Chemical"[MeSH Terms] OR "Chemical, Endocrine Disrupting"[MeSH Terms] OR "Disrupting Chemical, Endocrine"[MeSH Terms] OR "Endocrine Disruptor Effect"[MeSH Terms] OR "Endocrine Disruptor Effect"[MeSH Terms]OR "Water pollutants"[MeSH Terms] OR "Herbicides"[MeSH Terms] OR "Pesticides"[MeSH Terms] OR  "Gonadal Steroid Hormones"[MeSH Terms] OR "fertility"[MeSH Terms] OR "infertility"[MeSH Terms] OR "Androgen antagonists"[MeSH Terms] OR "astrogen antagonists"[MeSH Terms] OR "estrogen agonists"[MeSH Terms] OR "androgen agonists"[MeSH Terms]) </t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>6862</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>